<commit_message>
fixed sql related bugs
</commit_message>
<xml_diff>
--- a/stock_prediction_lstm/stock_prediction/config.xlsx
+++ b/stock_prediction_lstm/stock_prediction/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anon\PycharmProjects\stock_prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\PycharmProjects\memgpt\stocks\stocks\stock_prediction_lstm\stock_prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E838F6-6235-49F7-8D92-43799FB46761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23437AD7-3D3E-43DA-B7C6-E86FF33CD69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{3223D43E-ABA6-48AC-A435-0794344797E4}"/>
+    <workbookView xWindow="6195" yWindow="3015" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3223D43E-ABA6-48AC-A435-0794344797E4}"/>
   </bookViews>
   <sheets>
     <sheet name="script_config" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>HISTORY_TABLE</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>DATABASE</t>
+  </si>
+  <si>
+    <t>DATABASE_DRIVER</t>
+  </si>
+  <si>
+    <t>ODBC+Driver+11+for+SQL</t>
   </si>
 </sst>
 </file>
@@ -445,17 +451,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64720C97-430D-4B2C-8AF2-711F921FF766}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -463,7 +469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -471,7 +477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -479,7 +485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -487,7 +493,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -495,7 +501,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -503,7 +509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -511,7 +517,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -519,7 +525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -535,19 +541,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24046259-41C0-4FB7-BEAB-A49E4ABB996A}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -555,7 +561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -563,12 +569,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>